<commit_message>
feat(tools):added brave in broswer and utitlies such vlc ollama obs stuido notion
</commit_message>
<xml_diff>
--- a/public/tools.xlsx
+++ b/public/tools.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="259">
   <si>
     <t xml:space="preserve">category</t>
   </si>
@@ -572,6 +572,35 @@
     <t xml:space="preserve">brew install --cask microsoft-edge</t>
   </si>
   <si>
+    <t xml:space="preserve">Brave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choco install brave --pre </t>
+  </si>
+  <si>
+    <t xml:space="preserve">winget install --id=Brave.Brave  -e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scoop bucket add extras 
+scoop install extras/brave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo apt install curl
+sudo curl -fsSLo /usr/share/keyrings/brave-browser-archive-keyring.gpg https://brave-browser-apt-release.s3.brave.com/brave-browser-archive-keyring.gpg
+sudo curl -fsSLo /etc/apt/sources.list.d/brave-browser-release.sources https://brave-browser-apt-release.s3.brave.com/brave-browser.sources
+sudo apt update
+sudo apt install brave-browser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo dnf install dnf-plugins-core  sudo dnf config-manager addrepo --from-repofile=https://brave-browser-rpm-release.s3.brave.com/brave-browser.repo  sudo dnf install brave-browser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo pacman -Sy brave-browser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brew install --cask brave-browser</t>
+  </si>
+  <si>
     <t xml:space="preserve">DevOps</t>
   </si>
   <si>
@@ -614,7 +643,7 @@
     <t xml:space="preserve">sudo apt install kubectl</t>
   </si>
   <si>
-    <t xml:space="preserve">sudo dnf install kubectl</t>
+    <t xml:space="preserve">sudo dnf config-manager addrepo --from-repofile=https://brave-browser-rpm-release.s3.brave.com/brave-browser.repo</t>
   </si>
   <si>
     <t xml:space="preserve">sudo pacman -S kubectl</t>
@@ -665,7 +694,7 @@
     <t xml:space="preserve">sudo apt install nmap</t>
   </si>
   <si>
-    <t xml:space="preserve">sudo dnf install nmap</t>
+    <t xml:space="preserve">sudo dnf install brave-browser</t>
   </si>
   <si>
     <t xml:space="preserve">sudo pacman -S nmap</t>
@@ -696,6 +725,88 @@
   </si>
   <si>
     <t xml:space="preserve">brew install wireshark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vlc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choco install vlc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">winget install --id=VideoLAN.VLC  -e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scoop bucket add extras
+Scoop install extras/vlc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo apt install vlc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo dnf install vlc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo pacman -S vlc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brew install --cask vlc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obs studio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choco install obs-studio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">winget install --id=OBSProject.OBSStudio  -e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scoop bucket add extras
+scoop install extras/obs-studio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t: sudo apt install obs-studio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo dnf install obs-studio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo pacman -S obs-studio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choco install notion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">winget install --id=Notion.Notion  -e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scoop bucket add extras
+scoop install extras/notion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brew install --cask notion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ollama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choco install ollama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">winget install --id=Ollama.Ollama  -e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scoop bucket add main
+scoop install main/ollama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brew install ollama</t>
   </si>
 </sst>
 </file>
@@ -819,8 +930,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1495,38 +1606,38 @@
         <v>182</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="686.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>192</v>
@@ -1553,9 +1664,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>200</v>
@@ -1582,38 +1693,38 @@
         <v>207</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="G27" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="I27" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="I27" s="3" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
-        <v>208</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>217</v>
@@ -1640,7 +1751,130 @@
         <v>224</v>
       </c>
     </row>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>258</v>
+      </c>
+    </row>
     <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1721,11 +1955,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>